<commit_message>
:construction: Se modifica el servicio del login, list, create, read
</commit_message>
<xml_diff>
--- a/tests/data/testDataToken.xlsx
+++ b/tests/data/testDataToken.xlsx
@@ -11,12 +11,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>token</t>
   </si>
   <si>
-    <t>b0pkSdzKTDX2BtO4</t>
+    <t>status</t>
+  </si>
+  <si>
+    <t>GHsarcev7PR0pGK3</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>zwWNZF9j99XJPayu</t>
+  </si>
+  <si>
+    <t>JgClaIA3srPc11g3</t>
   </si>
 </sst>
 </file>
@@ -393,20 +405,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="1" max="2" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>